<commit_message>
Finished logical_design for student/course/registration database
</commit_message>
<xml_diff>
--- a/Module_4-Database_Design/M4_LogicalDesign_GregGarrett.xlsx
+++ b/Module_4-Database_Design/M4_LogicalDesign_GregGarrett.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\MSBA - Homework\Data Management and Organization (ANLY 6150)\Module 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\MSBA - Homework\Data Management and Organization (ANLY 6150)\Module_4-Database_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456DC512-C434-488C-938E-B8C4D07A3356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9664C80-D101-404E-88C5-EC6F7BF74577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-405" windowWidth="38640" windowHeight="21240" xr2:uid="{8E302556-DA7D-47B6-BD41-29498F706BD0}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="126">
   <si>
     <t>Requirements: Build a database to store student, course, and registration information</t>
   </si>
   <si>
-    <t>School</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>Course</t>
   </si>
   <si>
-    <t>Classroom Location</t>
-  </si>
-  <si>
     <t>Registration</t>
   </si>
   <si>
@@ -71,128 +65,362 @@
     <t>Billing</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Credits</t>
-  </si>
-  <si>
-    <t>Building Name</t>
-  </si>
-  <si>
-    <t>Classroom Number</t>
-  </si>
-  <si>
     <t>Capacity</t>
   </si>
   <si>
-    <t>Term Name</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Letter Grade</t>
-  </si>
-  <si>
-    <t>Numeric Grade</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
-    <t>Due Date</t>
-  </si>
-  <si>
-    <t>Payment Date</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Decription</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>School Id (PK)</t>
-  </si>
-  <si>
-    <t>Department Id (PK)</t>
-  </si>
-  <si>
-    <t>Teacher Id (PK)</t>
-  </si>
-  <si>
-    <t>Course Id (PK)</t>
-  </si>
-  <si>
-    <t>Classrom Id (PK)</t>
-  </si>
-  <si>
-    <t>Registration Id (PK)</t>
-  </si>
-  <si>
-    <t>Semester Id (PK)</t>
-  </si>
-  <si>
-    <t>Grade Id (PK)</t>
-  </si>
-  <si>
-    <t>Student Id (PK)</t>
-  </si>
-  <si>
-    <t>Billing Id (PK)</t>
-  </si>
-  <si>
-    <t>School Id (FK)</t>
-  </si>
-  <si>
     <t>Department Id (FK)</t>
   </si>
   <si>
-    <t>Teacher Id (FK)</t>
-  </si>
-  <si>
-    <t>Student Id (FK)</t>
-  </si>
-  <si>
-    <t>Course Id (FK)</t>
-  </si>
-  <si>
-    <t>Semester Id (FK)</t>
-  </si>
-  <si>
-    <t>Classroom Id (FK)</t>
-  </si>
-  <si>
-    <t>Letter Grade (FK)</t>
-  </si>
-  <si>
-    <t>Numeric Grade (FK)</t>
-  </si>
-  <si>
     <t>Amount (FK)</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Degree_Name</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Department_Id</t>
+  </si>
+  <si>
+    <t>Department_Id (FK)</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Department_Name</t>
+  </si>
+  <si>
+    <t>Teacher_First_Name</t>
+  </si>
+  <si>
+    <t>Phone_Number</t>
+  </si>
+  <si>
+    <t>Teacher_Last_Name</t>
+  </si>
+  <si>
+    <t>Course_Title</t>
+  </si>
+  <si>
+    <t>Number_Credits</t>
+  </si>
+  <si>
+    <t>Teacher_Id (FK)</t>
+  </si>
+  <si>
+    <t>Classroom_Id (FK)</t>
+  </si>
+  <si>
+    <t>Teacher_Id (PK)</t>
+  </si>
+  <si>
+    <t>Department_Id (PK)</t>
+  </si>
+  <si>
+    <t>Degree_Id (PK)</t>
+  </si>
+  <si>
+    <t>Course_Id (PK)</t>
+  </si>
+  <si>
+    <t>Semester_Id (PK)</t>
+  </si>
+  <si>
+    <t>Term_Availability</t>
+  </si>
+  <si>
+    <t>Classrom_Id (PK)</t>
+  </si>
+  <si>
+    <t>Building_Name</t>
+  </si>
+  <si>
+    <t>Classroom_Number</t>
+  </si>
+  <si>
+    <t>Grade_Id (PK)</t>
+  </si>
+  <si>
+    <t>Letter_Grade</t>
+  </si>
+  <si>
+    <t>Numeric_Grade</t>
+  </si>
+  <si>
+    <t>Student_Id (PK)</t>
+  </si>
+  <si>
+    <t>Billing_Id (PK)</t>
+  </si>
+  <si>
+    <t>Student_Id (FK)</t>
+  </si>
+  <si>
+    <t>Due_Date</t>
+  </si>
+  <si>
+    <t>Payment_Date</t>
+  </si>
+  <si>
+    <t>Registration_Id (PK)</t>
+  </si>
+  <si>
+    <t>Semester_Id (FK)</t>
+  </si>
+  <si>
+    <t>Course_Id (FK)</t>
+  </si>
+  <si>
+    <t>Letter_Grade (FK)</t>
+  </si>
+  <si>
+    <t>Numeric_Grade (FK)</t>
+  </si>
+  <si>
+    <t>Student_Degree</t>
+  </si>
+  <si>
+    <t>Student_Degree_Id</t>
+  </si>
+  <si>
+    <t>Degree_Id (FK)</t>
+  </si>
+  <si>
+    <t>Student_Degree_Id (PK)</t>
+  </si>
+  <si>
+    <t>Enrollment_Date</t>
+  </si>
+  <si>
+    <t>Graduation_Date</t>
+  </si>
+  <si>
+    <t>Degree_Id</t>
+  </si>
+  <si>
+    <t>Depatment_Id</t>
+  </si>
+  <si>
+    <t>Teacher_Id</t>
+  </si>
+  <si>
+    <t>Course_Id</t>
+  </si>
+  <si>
+    <t>Classroom_Id</t>
+  </si>
+  <si>
+    <t>Classroom_Location</t>
+  </si>
+  <si>
+    <t>Student_Id</t>
+  </si>
+  <si>
+    <t>Grade_Id</t>
+  </si>
+  <si>
+    <t>Registration_Id</t>
+  </si>
+  <si>
+    <t>Semester_Id</t>
+  </si>
+  <si>
+    <t>Billing_Id</t>
+  </si>
+  <si>
+    <t>deg0001</t>
+  </si>
+  <si>
+    <t>deg0002</t>
+  </si>
+  <si>
+    <t>business analytics</t>
+  </si>
+  <si>
+    <t>bachelor</t>
+  </si>
+  <si>
+    <t>dep0001</t>
+  </si>
+  <si>
+    <t>business</t>
+  </si>
+  <si>
+    <t>dep0002</t>
+  </si>
+  <si>
+    <t>biology</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>tch0001</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Olsen</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>tch0002</t>
+  </si>
+  <si>
+    <t>Hewitt</t>
+  </si>
+  <si>
+    <t>crs00001</t>
+  </si>
+  <si>
+    <t>data management</t>
+  </si>
+  <si>
+    <t>Database management and SQL queries</t>
+  </si>
+  <si>
+    <t>crs00002</t>
+  </si>
+  <si>
+    <t>developmental biology</t>
+  </si>
+  <si>
+    <t>Understanding life from conception to birth</t>
+  </si>
+  <si>
+    <t>Clancy School of Business</t>
+  </si>
+  <si>
+    <t>Campus</t>
+  </si>
+  <si>
+    <t>Einstein Science Building</t>
+  </si>
+  <si>
+    <t>clrmCSBR101</t>
+  </si>
+  <si>
+    <t>clrmESBR302</t>
+  </si>
+  <si>
+    <t>Campus &amp; Online</t>
+  </si>
+  <si>
+    <t>sem2024SP</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>sem2023AU</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>si000001</t>
+  </si>
+  <si>
+    <t>Becky</t>
+  </si>
+  <si>
+    <t>Palmer</t>
+  </si>
+  <si>
+    <t>becky_palmer@school.com</t>
+  </si>
+  <si>
+    <t>john_olsen@school.com</t>
+  </si>
+  <si>
+    <t>kate_hewitt@school.com</t>
+  </si>
+  <si>
+    <t>si000002</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Li</t>
+  </si>
+  <si>
+    <t>george_li@school.com</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>grd0001</t>
+  </si>
+  <si>
+    <t>grd0002</t>
+  </si>
+  <si>
+    <t>reg000001</t>
+  </si>
+  <si>
+    <t>reg00002</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>bil000001</t>
+  </si>
+  <si>
+    <t>bil000101</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Unpaid</t>
+  </si>
+  <si>
+    <t>sdg000001</t>
+  </si>
+  <si>
+    <t>sdg000002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,8 +436,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +458,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -246,11 +488,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -258,8 +523,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -333,15 +607,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1209675</xdr:colOff>
+      <xdr:colOff>1217295</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>17145</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -356,8 +630,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1847850" y="2085975"/>
-          <a:ext cx="1857375" cy="1581150"/>
+          <a:off x="1855470" y="2143125"/>
+          <a:ext cx="1857375" cy="1579245"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -387,8 +661,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1197428</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
@@ -396,7 +670,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>105455</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -410,9 +684,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3694339" y="3710668"/>
-          <a:ext cx="270102" cy="680"/>
+        <a:xfrm>
+          <a:off x="3800475" y="3724275"/>
+          <a:ext cx="257175" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -695,259 +969,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>131380</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>124811</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>131380</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="145" name="Straight Connector 144">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E52087C1-ED5E-D87B-2413-5C1398D5C615}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1859017" y="1602828"/>
-          <a:ext cx="124811" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>114601</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>122222</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>118110</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="147" name="Straight Connector 146">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14E26451-5D3D-D3E9-B611-BF9D8FC29E74}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1973881" y="1585262"/>
-          <a:ext cx="3509" cy="1664668"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>379095</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="149" name="Straight Connector 148">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5204B20F-A723-3B7E-BB3D-6AC5A71B2A95}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="379095" y="3242310"/>
-          <a:ext cx="1602105" cy="3810"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>389474</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>134138</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>394138</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>131379</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="151" name="Straight Connector 150">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A0CF268-AA41-DEA4-8850-133523E9E69E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="389474" y="3260966"/>
-          <a:ext cx="4664" cy="916896"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>385311</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>134335</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7423</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>134854</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="153" name="Straight Arrow Connector 152">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1FF66C4-AEE5-17A9-92BE-CCE587D066D8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="385311" y="4157695"/>
-          <a:ext cx="262192" cy="519"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>15</xdr:row>
@@ -1048,221 +1069,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>987137</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>73602</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>17318</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>106334</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="181" name="Connector: Elbow 180">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D1108D-8B59-4FE8-FF04-C1A6881D8E64}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7070148" y="619125"/>
-          <a:ext cx="1472045" cy="1305618"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 67398"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>121227</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>73602</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>991466</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>77932</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="185" name="Straight Connector 184">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18581A6C-68EC-B4D8-240B-9EB621547C9C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="1978602" y="619125"/>
-          <a:ext cx="5095875" cy="4330"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>113088</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>69272</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>116898</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>39486</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="187" name="Straight Connector 186">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25958752-8D21-219D-39FE-59ED1BBF3C3D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1970463" y="614795"/>
-          <a:ext cx="3810" cy="879418"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1216602</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>43296</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>121227</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>43296</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="189" name="Straight Connector 188">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8F2D9A0-E5D0-4DF3-4507-E4437BBCBA6F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1853045" y="1498023"/>
-          <a:ext cx="125557" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108239</xdr:rowOff>
+      <xdr:rowOff>99765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>138545</xdr:rowOff>
+      <xdr:rowOff>128166</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1277,8 +1093,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8524875" y="3926898"/>
-          <a:ext cx="1220932" cy="212147"/>
+          <a:off x="8533086" y="3962317"/>
+          <a:ext cx="1221828" cy="212332"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1308,16 +1124,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1219254</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>94731</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>8659</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>90921</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>8659</xdr:colOff>
+      <xdr:colOff>1219255</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>90921</xdr:rowOff>
+      <xdr:rowOff>94731</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1332,8 +1148,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8533534" y="3727739"/>
-          <a:ext cx="1220932" cy="181841"/>
+          <a:off x="8530513" y="3773352"/>
+          <a:ext cx="1221828" cy="183931"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1669,15 +1485,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>136072</xdr:colOff>
+      <xdr:colOff>133116</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>27214</xdr:rowOff>
+      <xdr:rowOff>28612</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>8474</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>87086</xdr:rowOff>
+      <xdr:rowOff>84674</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1692,8 +1508,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8665029" y="2901043"/>
-          <a:ext cx="1083128" cy="598714"/>
+          <a:off x="8662073" y="2902441"/>
+          <a:ext cx="1094558" cy="594904"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1726,13 +1542,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>21771</xdr:rowOff>
+      <xdr:rowOff>17961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>125186</xdr:colOff>
+      <xdr:colOff>154021</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>27214</xdr:rowOff>
+      <xdr:rowOff>28372</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1747,8 +1563,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="7500257" y="2895600"/>
-          <a:ext cx="1153886" cy="5443"/>
+          <a:off x="7494351" y="2936259"/>
+          <a:ext cx="1183532" cy="10411"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1873,16 +1689,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>10886</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1218929</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>43543</xdr:rowOff>
+      <xdr:rowOff>115661</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>21772</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>70757</xdr:rowOff>
+      <xdr:rowOff>119743</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1897,12 +1713,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9759043" y="1121229"/>
-          <a:ext cx="1208314" cy="206828"/>
+          <a:off x="9747886" y="1193347"/>
+          <a:ext cx="1241243" cy="183696"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 71138"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1929,15 +1745,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>5443</xdr:colOff>
+      <xdr:colOff>7075</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>130628</xdr:rowOff>
+      <xdr:rowOff>167095</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
+      <xdr:colOff>166823</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>130628</xdr:rowOff>
+      <xdr:rowOff>167095</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1952,8 +1768,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9753600" y="1208314"/>
-          <a:ext cx="157843" cy="0"/>
+          <a:off x="9755232" y="1244781"/>
+          <a:ext cx="159748" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1979,15 +1795,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>167096</xdr:colOff>
+      <xdr:colOff>168729</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>126818</xdr:rowOff>
+      <xdr:rowOff>163285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>167096</xdr:colOff>
+      <xdr:colOff>170906</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>90896</xdr:rowOff>
+      <xdr:rowOff>94706</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2002,8 +1818,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9915253" y="1204504"/>
-          <a:ext cx="0" cy="1400992"/>
+          <a:off x="9916886" y="1240971"/>
+          <a:ext cx="2177" cy="1368335"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2029,15 +1845,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>974272</xdr:colOff>
+      <xdr:colOff>970462</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>92529</xdr:rowOff>
+      <xdr:rowOff>83202</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>168729</xdr:colOff>
+      <xdr:colOff>172539</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>92529</xdr:rowOff>
+      <xdr:rowOff>83202</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2052,8 +1868,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9503229" y="2607129"/>
-          <a:ext cx="413657" cy="0"/>
+          <a:off x="9503548" y="2658236"/>
+          <a:ext cx="423905" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2079,15 +1895,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>968829</xdr:colOff>
+      <xdr:colOff>981113</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>103414</xdr:rowOff>
+      <xdr:rowOff>76285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>979714</xdr:colOff>
+      <xdr:colOff>988188</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>97972</xdr:rowOff>
+      <xdr:rowOff>57507</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2102,8 +1918,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9497786" y="2618014"/>
-          <a:ext cx="10885" cy="713015"/>
+          <a:off x="9514199" y="2651319"/>
+          <a:ext cx="7075" cy="716947"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2129,15 +1945,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>985157</xdr:colOff>
+      <xdr:colOff>988967</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>97972</xdr:rowOff>
+      <xdr:rowOff>67886</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>10886</xdr:colOff>
+      <xdr:colOff>8981</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>103414</xdr:rowOff>
+      <xdr:rowOff>79043</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2152,8 +1968,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9514114" y="3331029"/>
-          <a:ext cx="244929" cy="5442"/>
+          <a:off x="9522053" y="3378645"/>
+          <a:ext cx="241842" cy="11157"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2332,15 +2148,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1048839</xdr:colOff>
+      <xdr:colOff>1052649</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>119742</xdr:rowOff>
+      <xdr:rowOff>115931</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1050472</xdr:colOff>
+      <xdr:colOff>1052649</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>77833</xdr:rowOff>
+      <xdr:rowOff>77832</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2355,8 +2171,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9577796" y="4250871"/>
-          <a:ext cx="1633" cy="317319"/>
+          <a:off x="9585735" y="4346345"/>
+          <a:ext cx="0" cy="329763"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2382,15 +2198,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1055914</xdr:colOff>
+      <xdr:colOff>1044681</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>119742</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>5443</xdr:colOff>
+      <xdr:rowOff>96225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1210323</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>119742</xdr:rowOff>
+      <xdr:rowOff>96225</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2405,8 +2221,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9584871" y="4250871"/>
-          <a:ext cx="168729" cy="0"/>
+          <a:off x="9577767" y="4326639"/>
+          <a:ext cx="165642" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2414,6 +2230,569 @@
         <a:ln>
           <a:tailEnd type="triangle"/>
         </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1215258</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>216776</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F3BEBEC-0CD3-24B3-444F-6382BAF2720D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1852448" y="3704897"/>
+          <a:ext cx="223345" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>216776</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>52551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>216776</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>32845</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2CF3A6A-44D0-AB3D-9377-03D93554B5F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2075793" y="3179379"/>
+          <a:ext cx="0" cy="532087"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>59120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>229914</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>65689</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE407E89-739A-2175-031D-B4F0D03AC311}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="381000" y="3185948"/>
+          <a:ext cx="1707931" cy="6569"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>374431</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>118242</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>387569</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>78827</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38AE1E02-7D84-644E-C586-4C70CCF5F7BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="374431" y="2141483"/>
+          <a:ext cx="13138" cy="1064172"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>387569</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>111673</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>118242</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C1F8791-6BB4-C5F3-383C-43787D8D938D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="387569" y="2134914"/>
+          <a:ext cx="256190" cy="6569"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>262759</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>157655</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1095113</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>94725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Connector: Elbow 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B701674F-FDCF-FF3D-F178-438165AD3C86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2121776" y="525517"/>
+          <a:ext cx="10902578" cy="488863"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 97969"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>141514</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Connector: Elbow 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75D9B748-6FA8-CA7C-C593-0C3E00189DB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9889671" y="723900"/>
+          <a:ext cx="3135086" cy="458890"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 80400"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>272143</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>293915</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{561704DD-0FA2-4AC2-C39C-E1E4AB426E32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2128157" y="511629"/>
+          <a:ext cx="21772" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>293915</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E57A0B1E-C0F8-B700-7F7B-AF20BE0BCE3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1861457" y="1540329"/>
+          <a:ext cx="288472" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>141514</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>146957</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Connector 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20683E1C-969B-832C-D825-579990EA4ADB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9889671" y="723900"/>
+          <a:ext cx="5443" cy="391886"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Connector 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3199E1D-9771-1E2E-F547-D522F9DCF83C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9753600" y="1115786"/>
+          <a:ext cx="157843" cy="5443"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -2752,23 +3131,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB87B99-C53A-4003-A685-AB05DF1DCFCE}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="16.7890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.62890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.62890625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.47265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="16.7890625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.20703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="16.7890625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.62890625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.3125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1015625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.20703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.20703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.3125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7890625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.734375" customWidth="1"/>
+    <col min="16" max="16" width="10.20703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.26171875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.41796875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.15625" customWidth="1"/>
@@ -2780,217 +3162,817 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="M4" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="M5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="G6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="K6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E7" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="4" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1"/>
       <c r="E8" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>11</v>
+        <v>38</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="K12" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="J17" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="J18" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="F19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="J18" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="F19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="J19" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="D24" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="D25" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="D26" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" t="s">
+        <v>67</v>
+      </c>
+      <c r="K31" t="s">
+        <v>23</v>
+      </c>
+      <c r="L31" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" t="s">
+        <v>9</v>
+      </c>
+      <c r="N31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J32" t="s">
+        <v>103</v>
+      </c>
+      <c r="K32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L32" t="s">
+        <v>105</v>
+      </c>
+      <c r="M32" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="N32">
+        <v>8012230001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" t="s">
+        <v>78</v>
+      </c>
+      <c r="J33" t="s">
+        <v>109</v>
+      </c>
+      <c r="K33" t="s">
+        <v>110</v>
+      </c>
+      <c r="L33" t="s">
+        <v>111</v>
+      </c>
+      <c r="M33" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="N33">
+        <v>8012230002</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" t="s">
+        <v>43</v>
+      </c>
+      <c r="L36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37">
+        <v>8012221111</v>
+      </c>
+      <c r="J37" t="s">
+        <v>115</v>
+      </c>
+      <c r="K37" t="s">
+        <v>113</v>
+      </c>
+      <c r="L37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38">
+        <v>8012221112</v>
+      </c>
+      <c r="J38" t="s">
+        <v>116</v>
+      </c>
+      <c r="K38" t="s">
+        <v>114</v>
+      </c>
+      <c r="L38">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="J40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" t="s">
+        <v>27</v>
+      </c>
+      <c r="J41" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" t="s">
+        <v>67</v>
+      </c>
+      <c r="L41" t="s">
+        <v>70</v>
+      </c>
+      <c r="M41" t="s">
+        <v>64</v>
+      </c>
+      <c r="N41" t="s">
+        <v>43</v>
+      </c>
+      <c r="O41" t="s">
+        <v>44</v>
+      </c>
+      <c r="P41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42">
+        <v>8012221222</v>
+      </c>
+      <c r="J42" t="s">
+        <v>117</v>
+      </c>
+      <c r="K42" t="s">
+        <v>103</v>
+      </c>
+      <c r="L42" t="s">
+        <v>99</v>
+      </c>
+      <c r="M42" t="s">
+        <v>87</v>
+      </c>
+      <c r="N42" t="s">
+        <v>113</v>
+      </c>
+      <c r="O42">
+        <v>4</v>
+      </c>
+      <c r="P42">
+        <v>3432</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G43">
+        <v>8012221223</v>
+      </c>
+      <c r="J43" t="s">
+        <v>118</v>
+      </c>
+      <c r="K43" t="s">
+        <v>109</v>
+      </c>
+      <c r="L43" t="s">
+        <v>101</v>
+      </c>
+      <c r="M43" t="s">
+        <v>90</v>
+      </c>
+      <c r="N43" t="s">
+        <v>119</v>
+      </c>
+      <c r="O43">
+        <v>3.1</v>
+      </c>
+      <c r="P43">
+        <v>3432</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="J45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" t="s">
+        <v>63</v>
+      </c>
+      <c r="H46" t="s">
+        <v>65</v>
+      </c>
+      <c r="J46" t="s">
+        <v>71</v>
+      </c>
+      <c r="K46" t="s">
+        <v>67</v>
+      </c>
+      <c r="L46" t="s">
+        <v>12</v>
+      </c>
+      <c r="M46" t="s">
+        <v>48</v>
+      </c>
+      <c r="N46" t="s">
+        <v>49</v>
+      </c>
+      <c r="O46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" t="s">
+        <v>72</v>
+      </c>
+      <c r="G47" t="s">
+        <v>81</v>
+      </c>
+      <c r="J47" t="s">
+        <v>120</v>
+      </c>
+      <c r="K47" t="s">
+        <v>103</v>
+      </c>
+      <c r="L47">
+        <v>3432</v>
+      </c>
+      <c r="M47" s="11">
+        <v>44941</v>
+      </c>
+      <c r="N47" s="11">
+        <v>44940</v>
+      </c>
+      <c r="O47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48" t="s">
+        <v>85</v>
+      </c>
+      <c r="J48" t="s">
+        <v>121</v>
+      </c>
+      <c r="K48" t="s">
+        <v>103</v>
+      </c>
+      <c r="L48">
+        <v>3432</v>
+      </c>
+      <c r="M48" s="11">
+        <v>45672</v>
+      </c>
+      <c r="O48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" t="s">
+        <v>66</v>
+      </c>
+      <c r="J50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" t="s">
+        <v>56</v>
+      </c>
+      <c r="K51" t="s">
+        <v>61</v>
+      </c>
+      <c r="L51" t="s">
+        <v>67</v>
+      </c>
+      <c r="M51" t="s">
+        <v>59</v>
+      </c>
+      <c r="N51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52">
+        <v>101</v>
+      </c>
+      <c r="E52">
+        <v>54</v>
+      </c>
+      <c r="F52" t="s">
+        <v>94</v>
+      </c>
+      <c r="J52" t="s">
+        <v>124</v>
+      </c>
+      <c r="K52" t="s">
+        <v>72</v>
+      </c>
+      <c r="L52" t="s">
+        <v>103</v>
+      </c>
+      <c r="M52" s="11">
+        <v>44927</v>
+      </c>
+      <c r="N52" s="11">
+        <v>46737</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53">
+        <v>302</v>
+      </c>
+      <c r="E53">
         <v>32</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="2" t="s">
+      <c r="F53" t="s">
+        <v>98</v>
+      </c>
+      <c r="J53" t="s">
+        <v>125</v>
+      </c>
+      <c r="K53" t="s">
+        <v>73</v>
+      </c>
+      <c r="L53" t="s">
+        <v>109</v>
+      </c>
+      <c r="M53" s="11">
+        <v>44713</v>
+      </c>
+      <c r="N53" s="11">
+        <v>46143</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>49</v>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" t="s">
+        <v>102</v>
+      </c>
+      <c r="D58">
+        <v>2023</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F42" r:id="rId1" xr:uid="{09D26A75-8967-45CF-A061-BE435DDAA5A9}"/>
+    <hyperlink ref="F43" r:id="rId2" xr:uid="{1753893A-BCAA-47D5-AF96-CD839E50EF95}"/>
+    <hyperlink ref="M32" r:id="rId3" xr:uid="{CBB63535-470C-4648-B016-AE7905360655}"/>
+    <hyperlink ref="M33" r:id="rId4" xr:uid="{4358CFF9-2DAB-43F0-B789-4CEB1CA625CB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed billing description from  billing table
</commit_message>
<xml_diff>
--- a/Module_4-Database_Design/M4_LogicalDesign_GregGarrett.xlsx
+++ b/Module_4-Database_Design/M4_LogicalDesign_GregGarrett.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\MSBA - Homework\Data Management and Organization (ANLY 6150)\Module 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\MSBA - Homework\Data Management and Organization (ANLY 6150)\Module_4-Database_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456DC512-C434-488C-938E-B8C4D07A3356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC862B11-A6FC-447C-B610-ECCB867A1A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-405" windowWidth="38640" windowHeight="21240" xr2:uid="{8E302556-DA7D-47B6-BD41-29498F706BD0}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="126">
   <si>
     <t>Requirements: Build a database to store student, course, and registration information</t>
   </si>
   <si>
-    <t>School</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>Course</t>
   </si>
   <si>
-    <t>Classroom Location</t>
-  </si>
-  <si>
     <t>Registration</t>
   </si>
   <si>
@@ -71,128 +65,362 @@
     <t>Billing</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Credits</t>
-  </si>
-  <si>
-    <t>Building Name</t>
-  </si>
-  <si>
-    <t>Classroom Number</t>
-  </si>
-  <si>
     <t>Capacity</t>
   </si>
   <si>
-    <t>Term Name</t>
-  </si>
-  <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Letter Grade</t>
-  </si>
-  <si>
-    <t>Numeric Grade</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
-    <t>Due Date</t>
-  </si>
-  <si>
-    <t>Payment Date</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Decription</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>School Id (PK)</t>
-  </si>
-  <si>
-    <t>Department Id (PK)</t>
-  </si>
-  <si>
-    <t>Teacher Id (PK)</t>
-  </si>
-  <si>
-    <t>Course Id (PK)</t>
-  </si>
-  <si>
-    <t>Classrom Id (PK)</t>
-  </si>
-  <si>
-    <t>Registration Id (PK)</t>
-  </si>
-  <si>
-    <t>Semester Id (PK)</t>
-  </si>
-  <si>
-    <t>Grade Id (PK)</t>
-  </si>
-  <si>
-    <t>Student Id (PK)</t>
-  </si>
-  <si>
-    <t>Billing Id (PK)</t>
-  </si>
-  <si>
-    <t>School Id (FK)</t>
-  </si>
-  <si>
     <t>Department Id (FK)</t>
   </si>
   <si>
-    <t>Teacher Id (FK)</t>
-  </si>
-  <si>
-    <t>Student Id (FK)</t>
-  </si>
-  <si>
-    <t>Course Id (FK)</t>
-  </si>
-  <si>
-    <t>Semester Id (FK)</t>
-  </si>
-  <si>
-    <t>Classroom Id (FK)</t>
-  </si>
-  <si>
-    <t>Letter Grade (FK)</t>
-  </si>
-  <si>
-    <t>Numeric Grade (FK)</t>
-  </si>
-  <si>
     <t>Amount (FK)</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Degree_Name</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Department_Id</t>
+  </si>
+  <si>
+    <t>Department_Id (FK)</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
+  </si>
+  <si>
+    <t>Department_Name</t>
+  </si>
+  <si>
+    <t>Teacher_First_Name</t>
+  </si>
+  <si>
+    <t>Phone_Number</t>
+  </si>
+  <si>
+    <t>Teacher_Last_Name</t>
+  </si>
+  <si>
+    <t>Course_Title</t>
+  </si>
+  <si>
+    <t>Number_Credits</t>
+  </si>
+  <si>
+    <t>Teacher_Id (FK)</t>
+  </si>
+  <si>
+    <t>Classroom_Id (FK)</t>
+  </si>
+  <si>
+    <t>Teacher_Id (PK)</t>
+  </si>
+  <si>
+    <t>Department_Id (PK)</t>
+  </si>
+  <si>
+    <t>Degree_Id (PK)</t>
+  </si>
+  <si>
+    <t>Course_Id (PK)</t>
+  </si>
+  <si>
+    <t>Semester_Id (PK)</t>
+  </si>
+  <si>
+    <t>Term_Availability</t>
+  </si>
+  <si>
+    <t>Classrom_Id (PK)</t>
+  </si>
+  <si>
+    <t>Building_Name</t>
+  </si>
+  <si>
+    <t>Classroom_Number</t>
+  </si>
+  <si>
+    <t>Grade_Id (PK)</t>
+  </si>
+  <si>
+    <t>Letter_Grade</t>
+  </si>
+  <si>
+    <t>Numeric_Grade</t>
+  </si>
+  <si>
+    <t>Student_Id (PK)</t>
+  </si>
+  <si>
+    <t>Billing_Id (PK)</t>
+  </si>
+  <si>
+    <t>Student_Id (FK)</t>
+  </si>
+  <si>
+    <t>Due_Date</t>
+  </si>
+  <si>
+    <t>Payment_Date</t>
+  </si>
+  <si>
+    <t>Registration_Id (PK)</t>
+  </si>
+  <si>
+    <t>Semester_Id (FK)</t>
+  </si>
+  <si>
+    <t>Course_Id (FK)</t>
+  </si>
+  <si>
+    <t>Letter_Grade (FK)</t>
+  </si>
+  <si>
+    <t>Numeric_Grade (FK)</t>
+  </si>
+  <si>
+    <t>Student_Degree</t>
+  </si>
+  <si>
+    <t>Student_Degree_Id</t>
+  </si>
+  <si>
+    <t>Degree_Id (FK)</t>
+  </si>
+  <si>
+    <t>Student_Degree_Id (PK)</t>
+  </si>
+  <si>
+    <t>Enrollment_Date</t>
+  </si>
+  <si>
+    <t>Graduation_Date</t>
+  </si>
+  <si>
+    <t>Degree_Id</t>
+  </si>
+  <si>
+    <t>Depatment_Id</t>
+  </si>
+  <si>
+    <t>Teacher_Id</t>
+  </si>
+  <si>
+    <t>Course_Id</t>
+  </si>
+  <si>
+    <t>Classroom_Id</t>
+  </si>
+  <si>
+    <t>Classroom_Location</t>
+  </si>
+  <si>
+    <t>Student_Id</t>
+  </si>
+  <si>
+    <t>Grade_Id</t>
+  </si>
+  <si>
+    <t>Registration_Id</t>
+  </si>
+  <si>
+    <t>Semester_Id</t>
+  </si>
+  <si>
+    <t>Billing_Id</t>
+  </si>
+  <si>
+    <t>deg0001</t>
+  </si>
+  <si>
+    <t>deg0002</t>
+  </si>
+  <si>
+    <t>business analytics</t>
+  </si>
+  <si>
+    <t>bachelor</t>
+  </si>
+  <si>
+    <t>dep0001</t>
+  </si>
+  <si>
+    <t>business</t>
+  </si>
+  <si>
+    <t>dep0002</t>
+  </si>
+  <si>
+    <t>biology</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>tch0001</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Olsen</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>tch0002</t>
+  </si>
+  <si>
+    <t>Hewitt</t>
+  </si>
+  <si>
+    <t>crs00001</t>
+  </si>
+  <si>
+    <t>data management</t>
+  </si>
+  <si>
+    <t>Database management and SQL queries</t>
+  </si>
+  <si>
+    <t>crs00002</t>
+  </si>
+  <si>
+    <t>developmental biology</t>
+  </si>
+  <si>
+    <t>Understanding life from conception to birth</t>
+  </si>
+  <si>
+    <t>Clancy School of Business</t>
+  </si>
+  <si>
+    <t>Campus</t>
+  </si>
+  <si>
+    <t>Einstein Science Building</t>
+  </si>
+  <si>
+    <t>clrmCSBR101</t>
+  </si>
+  <si>
+    <t>clrmESBR302</t>
+  </si>
+  <si>
+    <t>Campus &amp; Online</t>
+  </si>
+  <si>
+    <t>sem2024SP</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>sem2023AU</t>
+  </si>
+  <si>
+    <t>Autumn</t>
+  </si>
+  <si>
+    <t>si000001</t>
+  </si>
+  <si>
+    <t>Becky</t>
+  </si>
+  <si>
+    <t>Palmer</t>
+  </si>
+  <si>
+    <t>becky_palmer@school.com</t>
+  </si>
+  <si>
+    <t>john_olsen@school.com</t>
+  </si>
+  <si>
+    <t>kate_hewitt@school.com</t>
+  </si>
+  <si>
+    <t>si000002</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Li</t>
+  </si>
+  <si>
+    <t>george_li@school.com</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>grd0001</t>
+  </si>
+  <si>
+    <t>grd0002</t>
+  </si>
+  <si>
+    <t>reg000001</t>
+  </si>
+  <si>
+    <t>reg00002</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>bil000001</t>
+  </si>
+  <si>
+    <t>bil000101</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Unpaid</t>
+  </si>
+  <si>
+    <t>sdg000001</t>
+  </si>
+  <si>
+    <t>sdg000002</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,8 +436,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +458,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -246,11 +488,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -258,8 +523,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -333,15 +607,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1209675</xdr:colOff>
+      <xdr:colOff>1217295</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>17145</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -356,8 +630,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1847850" y="2085975"/>
-          <a:ext cx="1857375" cy="1581150"/>
+          <a:off x="1855470" y="2143125"/>
+          <a:ext cx="1857375" cy="1579245"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -387,8 +661,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1197428</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
@@ -396,7 +670,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>105455</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -410,9 +684,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3694339" y="3710668"/>
-          <a:ext cx="270102" cy="680"/>
+        <a:xfrm>
+          <a:off x="3800475" y="3724275"/>
+          <a:ext cx="257175" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -695,259 +969,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>131380</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>124811</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>131380</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="145" name="Straight Connector 144">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E52087C1-ED5E-D87B-2413-5C1398D5C615}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1859017" y="1602828"/>
-          <a:ext cx="124811" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>114601</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>122222</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>118110</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="147" name="Straight Connector 146">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14E26451-5D3D-D3E9-B611-BF9D8FC29E74}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1973881" y="1585262"/>
-          <a:ext cx="3509" cy="1664668"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>379095</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="149" name="Straight Connector 148">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5204B20F-A723-3B7E-BB3D-6AC5A71B2A95}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="379095" y="3242310"/>
-          <a:ext cx="1602105" cy="3810"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>389474</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>134138</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>394138</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>131379</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="151" name="Straight Connector 150">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A0CF268-AA41-DEA4-8850-133523E9E69E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="389474" y="3260966"/>
-          <a:ext cx="4664" cy="916896"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>385311</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>134335</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7423</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>134854</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="153" name="Straight Arrow Connector 152">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1FF66C4-AEE5-17A9-92BE-CCE587D066D8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="385311" y="4157695"/>
-          <a:ext cx="262192" cy="519"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>15</xdr:row>
@@ -1048,221 +1069,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>987137</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>73602</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>17318</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>106334</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="181" name="Connector: Elbow 180">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D1108D-8B59-4FE8-FF04-C1A6881D8E64}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7070148" y="619125"/>
-          <a:ext cx="1472045" cy="1305618"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 67398"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>121227</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>73602</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>991466</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>77932</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="185" name="Straight Connector 184">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18581A6C-68EC-B4D8-240B-9EB621547C9C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="1978602" y="619125"/>
-          <a:ext cx="5095875" cy="4330"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>113088</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>69272</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>116898</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>39486</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="187" name="Straight Connector 186">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25958752-8D21-219D-39FE-59ED1BBF3C3D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1970463" y="614795"/>
-          <a:ext cx="3810" cy="879418"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1216602</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>43296</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>121227</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>43296</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="189" name="Straight Connector 188">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8F2D9A0-E5D0-4DF3-4507-E4437BBCBA6F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1853045" y="1498023"/>
-          <a:ext cx="125557" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108239</xdr:rowOff>
+      <xdr:rowOff>99765</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>138545</xdr:rowOff>
+      <xdr:rowOff>128166</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1277,8 +1093,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8524875" y="3926898"/>
-          <a:ext cx="1220932" cy="212147"/>
+          <a:off x="8533086" y="3962317"/>
+          <a:ext cx="1221828" cy="212332"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1308,16 +1124,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1219254</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>94731</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>8659</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>90921</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>8659</xdr:colOff>
+      <xdr:colOff>1219255</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>90921</xdr:rowOff>
+      <xdr:rowOff>94731</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1332,8 +1148,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8533534" y="3727739"/>
-          <a:ext cx="1220932" cy="181841"/>
+          <a:off x="8530513" y="3773352"/>
+          <a:ext cx="1221828" cy="183931"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1669,15 +1485,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>136072</xdr:colOff>
+      <xdr:colOff>133116</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>27214</xdr:rowOff>
+      <xdr:rowOff>28612</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>8474</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>87086</xdr:rowOff>
+      <xdr:rowOff>84674</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1692,8 +1508,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8665029" y="2901043"/>
-          <a:ext cx="1083128" cy="598714"/>
+          <a:off x="8662073" y="2902441"/>
+          <a:ext cx="1094558" cy="594904"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1726,13 +1542,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>21771</xdr:rowOff>
+      <xdr:rowOff>17961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>125186</xdr:colOff>
+      <xdr:colOff>154021</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>27214</xdr:rowOff>
+      <xdr:rowOff>28372</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1747,8 +1563,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="7500257" y="2895600"/>
-          <a:ext cx="1153886" cy="5443"/>
+          <a:off x="7494351" y="2936259"/>
+          <a:ext cx="1183532" cy="10411"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1873,16 +1689,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>10886</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1218929</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>43543</xdr:rowOff>
+      <xdr:rowOff>115661</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>21772</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>70757</xdr:rowOff>
+      <xdr:rowOff>119743</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1897,12 +1713,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9759043" y="1121229"/>
-          <a:ext cx="1208314" cy="206828"/>
+          <a:off x="9747886" y="1193347"/>
+          <a:ext cx="1241243" cy="183696"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 71138"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1929,15 +1745,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>5443</xdr:colOff>
+      <xdr:colOff>7075</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>130628</xdr:rowOff>
+      <xdr:rowOff>167095</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
+      <xdr:colOff>166823</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>130628</xdr:rowOff>
+      <xdr:rowOff>167095</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1952,8 +1768,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9753600" y="1208314"/>
-          <a:ext cx="157843" cy="0"/>
+          <a:off x="9755232" y="1244781"/>
+          <a:ext cx="159748" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1979,15 +1795,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>167096</xdr:colOff>
+      <xdr:colOff>168729</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>126818</xdr:rowOff>
+      <xdr:rowOff>163285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>167096</xdr:colOff>
+      <xdr:colOff>170906</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>90896</xdr:rowOff>
+      <xdr:rowOff>94706</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2002,8 +1818,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9915253" y="1204504"/>
-          <a:ext cx="0" cy="1400992"/>
+          <a:off x="9916886" y="1240971"/>
+          <a:ext cx="2177" cy="1368335"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2029,15 +1845,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>974272</xdr:colOff>
+      <xdr:colOff>970462</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>92529</xdr:rowOff>
+      <xdr:rowOff>83202</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>168729</xdr:colOff>
+      <xdr:colOff>172539</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>92529</xdr:rowOff>
+      <xdr:rowOff>83202</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2052,8 +1868,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9503229" y="2607129"/>
-          <a:ext cx="413657" cy="0"/>
+          <a:off x="9503548" y="2658236"/>
+          <a:ext cx="423905" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2079,15 +1895,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>968829</xdr:colOff>
+      <xdr:colOff>981113</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>103414</xdr:rowOff>
+      <xdr:rowOff>76285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>979714</xdr:colOff>
+      <xdr:colOff>988188</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>97972</xdr:rowOff>
+      <xdr:rowOff>57507</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2102,8 +1918,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9497786" y="2618014"/>
-          <a:ext cx="10885" cy="713015"/>
+          <a:off x="9514199" y="2651319"/>
+          <a:ext cx="7075" cy="716947"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2129,15 +1945,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>985157</xdr:colOff>
+      <xdr:colOff>988967</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>97972</xdr:rowOff>
+      <xdr:rowOff>67886</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>10886</xdr:colOff>
+      <xdr:colOff>8981</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>103414</xdr:rowOff>
+      <xdr:rowOff>79043</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2152,8 +1968,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9514114" y="3331029"/>
-          <a:ext cx="244929" cy="5442"/>
+          <a:off x="9522053" y="3378645"/>
+          <a:ext cx="241842" cy="11157"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2332,15 +2148,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1048839</xdr:colOff>
+      <xdr:colOff>1052649</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>119742</xdr:rowOff>
+      <xdr:rowOff>115931</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1050472</xdr:colOff>
+      <xdr:colOff>1052649</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>77833</xdr:rowOff>
+      <xdr:rowOff>77832</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2355,8 +2171,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9577796" y="4250871"/>
-          <a:ext cx="1633" cy="317319"/>
+          <a:off x="9585735" y="4346345"/>
+          <a:ext cx="0" cy="329763"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2382,15 +2198,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1055914</xdr:colOff>
+      <xdr:colOff>1044681</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>119742</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>5443</xdr:colOff>
+      <xdr:rowOff>96225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1210323</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>119742</xdr:rowOff>
+      <xdr:rowOff>96225</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2405,8 +2221,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9584871" y="4250871"/>
-          <a:ext cx="168729" cy="0"/>
+          <a:off x="9577767" y="4326639"/>
+          <a:ext cx="165642" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2414,6 +2230,569 @@
         <a:ln>
           <a:tailEnd type="triangle"/>
         </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1215258</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>216776</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F3BEBEC-0CD3-24B3-444F-6382BAF2720D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1852448" y="3704897"/>
+          <a:ext cx="223345" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>216776</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>52551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>216776</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>32845</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2CF3A6A-44D0-AB3D-9377-03D93554B5F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2075793" y="3179379"/>
+          <a:ext cx="0" cy="532087"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>59120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>229914</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>65689</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE407E89-739A-2175-031D-B4F0D03AC311}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="381000" y="3185948"/>
+          <a:ext cx="1707931" cy="6569"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>374431</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>118242</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>387569</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>78827</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38AE1E02-7D84-644E-C586-4C70CCF5F7BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="374431" y="2141483"/>
+          <a:ext cx="13138" cy="1064172"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>387569</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>111673</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>118242</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C1F8791-6BB4-C5F3-383C-43787D8D938D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="387569" y="2134914"/>
+          <a:ext cx="256190" cy="6569"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>262759</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>157655</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1095113</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>94725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Connector: Elbow 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B701674F-FDCF-FF3D-F178-438165AD3C86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2121776" y="525517"/>
+          <a:ext cx="10902578" cy="488863"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 97969"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>141514</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Connector: Elbow 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75D9B748-6FA8-CA7C-C593-0C3E00189DB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9889671" y="723900"/>
+          <a:ext cx="3135086" cy="458890"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 80400"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>272143</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>293915</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{561704DD-0FA2-4AC2-C39C-E1E4AB426E32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2128157" y="511629"/>
+          <a:ext cx="21772" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>293915</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E57A0B1E-C0F8-B700-7F7B-AF20BE0BCE3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1861457" y="1540329"/>
+          <a:ext cx="288472" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>141514</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>146957</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Connector 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20683E1C-969B-832C-D825-579990EA4ADB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9889671" y="723900"/>
+          <a:ext cx="5443" cy="391886"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Connector 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3199E1D-9771-1E2E-F547-D522F9DCF83C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9753600" y="1115786"/>
+          <a:ext cx="157843" cy="5443"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -2752,23 +3131,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB87B99-C53A-4003-A685-AB05DF1DCFCE}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="16.7890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="16.62890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.83984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.62890625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.47265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="16.7890625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.20703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="16.7890625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.62890625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.3125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1015625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.20703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.20703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.3125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7890625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.734375" customWidth="1"/>
+    <col min="16" max="16" width="10.20703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.26171875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.41796875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8.15625" customWidth="1"/>
@@ -2780,217 +3162,817 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="M4" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="M5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="G6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="K6" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E7" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="4" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1"/>
       <c r="E8" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>11</v>
+        <v>38</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="E12" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="K12" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="E14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="J17" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="J18" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="F19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="J18" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="F19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="J19" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="D24" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="D25" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="D26" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" t="s">
+        <v>67</v>
+      </c>
+      <c r="K31" t="s">
+        <v>23</v>
+      </c>
+      <c r="L31" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" t="s">
+        <v>9</v>
+      </c>
+      <c r="N31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" t="s">
+        <v>76</v>
+      </c>
+      <c r="J32" t="s">
+        <v>103</v>
+      </c>
+      <c r="K32" t="s">
+        <v>104</v>
+      </c>
+      <c r="L32" t="s">
+        <v>105</v>
+      </c>
+      <c r="M32" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="N32">
+        <v>8012230001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" t="s">
+        <v>78</v>
+      </c>
+      <c r="J33" t="s">
+        <v>109</v>
+      </c>
+      <c r="K33" t="s">
+        <v>110</v>
+      </c>
+      <c r="L33" t="s">
+        <v>111</v>
+      </c>
+      <c r="M33" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="N33">
+        <v>8012230002</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" t="s">
+        <v>43</v>
+      </c>
+      <c r="L36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37">
+        <v>8012221111</v>
+      </c>
+      <c r="J37" t="s">
+        <v>115</v>
+      </c>
+      <c r="K37" t="s">
+        <v>113</v>
+      </c>
+      <c r="L37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38">
+        <v>8012221112</v>
+      </c>
+      <c r="J38" t="s">
+        <v>116</v>
+      </c>
+      <c r="K38" t="s">
+        <v>114</v>
+      </c>
+      <c r="L38">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="J40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" t="s">
+        <v>27</v>
+      </c>
+      <c r="J41" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" t="s">
+        <v>67</v>
+      </c>
+      <c r="L41" t="s">
+        <v>70</v>
+      </c>
+      <c r="M41" t="s">
+        <v>64</v>
+      </c>
+      <c r="N41" t="s">
+        <v>43</v>
+      </c>
+      <c r="O41" t="s">
+        <v>44</v>
+      </c>
+      <c r="P41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G42">
+        <v>8012221222</v>
+      </c>
+      <c r="J42" t="s">
+        <v>117</v>
+      </c>
+      <c r="K42" t="s">
+        <v>103</v>
+      </c>
+      <c r="L42" t="s">
+        <v>99</v>
+      </c>
+      <c r="M42" t="s">
+        <v>87</v>
+      </c>
+      <c r="N42" t="s">
+        <v>113</v>
+      </c>
+      <c r="O42">
+        <v>4</v>
+      </c>
+      <c r="P42">
+        <v>3432</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" t="s">
+        <v>78</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G43">
+        <v>8012221223</v>
+      </c>
+      <c r="J43" t="s">
+        <v>118</v>
+      </c>
+      <c r="K43" t="s">
+        <v>109</v>
+      </c>
+      <c r="L43" t="s">
+        <v>101</v>
+      </c>
+      <c r="M43" t="s">
+        <v>90</v>
+      </c>
+      <c r="N43" t="s">
+        <v>119</v>
+      </c>
+      <c r="O43">
+        <v>3.1</v>
+      </c>
+      <c r="P43">
+        <v>3432</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="J45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" t="s">
+        <v>30</v>
+      </c>
+      <c r="E46" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" t="s">
+        <v>63</v>
+      </c>
+      <c r="H46" t="s">
+        <v>65</v>
+      </c>
+      <c r="J46" t="s">
+        <v>71</v>
+      </c>
+      <c r="K46" t="s">
+        <v>67</v>
+      </c>
+      <c r="L46" t="s">
+        <v>12</v>
+      </c>
+      <c r="M46" t="s">
+        <v>48</v>
+      </c>
+      <c r="N46" t="s">
+        <v>49</v>
+      </c>
+      <c r="O46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" t="s">
+        <v>72</v>
+      </c>
+      <c r="G47" t="s">
+        <v>81</v>
+      </c>
+      <c r="J47" t="s">
+        <v>120</v>
+      </c>
+      <c r="K47" t="s">
+        <v>103</v>
+      </c>
+      <c r="L47">
+        <v>3432</v>
+      </c>
+      <c r="M47" s="11">
+        <v>44941</v>
+      </c>
+      <c r="N47" s="11">
+        <v>44940</v>
+      </c>
+      <c r="O47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>92</v>
+      </c>
+      <c r="F48" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48" t="s">
+        <v>85</v>
+      </c>
+      <c r="J48" t="s">
+        <v>121</v>
+      </c>
+      <c r="K48" t="s">
+        <v>103</v>
+      </c>
+      <c r="L48">
+        <v>3432</v>
+      </c>
+      <c r="M48" s="11">
+        <v>45672</v>
+      </c>
+      <c r="O48" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B50" t="s">
+        <v>66</v>
+      </c>
+      <c r="J50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" t="s">
+        <v>17</v>
+      </c>
+      <c r="J51" t="s">
+        <v>56</v>
+      </c>
+      <c r="K51" t="s">
+        <v>61</v>
+      </c>
+      <c r="L51" t="s">
+        <v>67</v>
+      </c>
+      <c r="M51" t="s">
+        <v>59</v>
+      </c>
+      <c r="N51" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52">
+        <v>101</v>
+      </c>
+      <c r="E52">
+        <v>54</v>
+      </c>
+      <c r="F52" t="s">
+        <v>94</v>
+      </c>
+      <c r="J52" t="s">
+        <v>124</v>
+      </c>
+      <c r="K52" t="s">
+        <v>72</v>
+      </c>
+      <c r="L52" t="s">
+        <v>103</v>
+      </c>
+      <c r="M52" s="11">
+        <v>44927</v>
+      </c>
+      <c r="N52" s="11">
+        <v>46737</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D53">
+        <v>302</v>
+      </c>
+      <c r="E53">
         <v>32</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="2" t="s">
+      <c r="F53" t="s">
+        <v>98</v>
+      </c>
+      <c r="J53" t="s">
+        <v>125</v>
+      </c>
+      <c r="K53" t="s">
+        <v>73</v>
+      </c>
+      <c r="L53" t="s">
+        <v>109</v>
+      </c>
+      <c r="M53" s="11">
+        <v>44713</v>
+      </c>
+      <c r="N53" s="11">
+        <v>46143</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>49</v>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" t="s">
+        <v>102</v>
+      </c>
+      <c r="D58">
+        <v>2023</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F42" r:id="rId1" xr:uid="{09D26A75-8967-45CF-A061-BE435DDAA5A9}"/>
+    <hyperlink ref="F43" r:id="rId2" xr:uid="{1753893A-BCAA-47D5-AF96-CD839E50EF95}"/>
+    <hyperlink ref="M32" r:id="rId3" xr:uid="{CBB63535-470C-4648-B016-AE7905360655}"/>
+    <hyperlink ref="M33" r:id="rId4" xr:uid="{4358CFF9-2DAB-43F0-B789-4CEB1CA625CB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished creating documentation for M4 database creation
</commit_message>
<xml_diff>
--- a/Module_4-Database_Design/M4_LogicalDesign_GregGarrett.xlsx
+++ b/Module_4-Database_Design/M4_LogicalDesign_GregGarrett.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\MSBA - Homework\Data Management and Organization (ANLY 6150)\Module_4-Database_Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i58993\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC862B11-A6FC-447C-B610-ECCB867A1A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B222BF-D9D3-47C8-863F-A1CF7138B444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-405" windowWidth="38640" windowHeight="21240" xr2:uid="{8E302556-DA7D-47B6-BD41-29498F706BD0}"/>
+    <workbookView xWindow="57480" yWindow="-405" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{8E302556-DA7D-47B6-BD41-29498F706BD0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Logical Database Design" sheetId="1" r:id="rId1"/>
+    <sheet name="Physical Database Design" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="144">
   <si>
     <t>Requirements: Build a database to store student, course, and registration information</t>
   </si>
@@ -83,12 +84,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Department Id (FK)</t>
-  </si>
-  <si>
-    <t>Amount (FK)</t>
-  </si>
-  <si>
     <t>Style</t>
   </si>
   <si>
@@ -104,9 +99,6 @@
     <t>Department_Id</t>
   </si>
   <si>
-    <t>Department_Id (FK)</t>
-  </si>
-  <si>
     <t>First_Name</t>
   </si>
   <si>
@@ -131,90 +123,33 @@
     <t>Number_Credits</t>
   </si>
   <si>
-    <t>Teacher_Id (FK)</t>
-  </si>
-  <si>
-    <t>Classroom_Id (FK)</t>
-  </si>
-  <si>
-    <t>Teacher_Id (PK)</t>
-  </si>
-  <si>
-    <t>Department_Id (PK)</t>
-  </si>
-  <si>
-    <t>Degree_Id (PK)</t>
-  </si>
-  <si>
-    <t>Course_Id (PK)</t>
-  </si>
-  <si>
-    <t>Semester_Id (PK)</t>
-  </si>
-  <si>
     <t>Term_Availability</t>
   </si>
   <si>
-    <t>Classrom_Id (PK)</t>
-  </si>
-  <si>
     <t>Building_Name</t>
   </si>
   <si>
     <t>Classroom_Number</t>
   </si>
   <si>
-    <t>Grade_Id (PK)</t>
-  </si>
-  <si>
     <t>Letter_Grade</t>
   </si>
   <si>
     <t>Numeric_Grade</t>
   </si>
   <si>
-    <t>Student_Id (PK)</t>
-  </si>
-  <si>
-    <t>Billing_Id (PK)</t>
-  </si>
-  <si>
-    <t>Student_Id (FK)</t>
-  </si>
-  <si>
     <t>Due_Date</t>
   </si>
   <si>
     <t>Payment_Date</t>
   </si>
   <si>
-    <t>Registration_Id (PK)</t>
-  </si>
-  <si>
-    <t>Semester_Id (FK)</t>
-  </si>
-  <si>
-    <t>Course_Id (FK)</t>
-  </si>
-  <si>
-    <t>Letter_Grade (FK)</t>
-  </si>
-  <si>
-    <t>Numeric_Grade (FK)</t>
-  </si>
-  <si>
     <t>Student_Degree</t>
   </si>
   <si>
     <t>Student_Degree_Id</t>
   </si>
   <si>
-    <t>Degree_Id (FK)</t>
-  </si>
-  <si>
-    <t>Student_Degree_Id (PK)</t>
-  </si>
-  <si>
     <t>Enrollment_Date</t>
   </si>
   <si>
@@ -254,36 +189,6 @@
     <t>Billing_Id</t>
   </si>
   <si>
-    <t>deg0001</t>
-  </si>
-  <si>
-    <t>deg0002</t>
-  </si>
-  <si>
-    <t>business analytics</t>
-  </si>
-  <si>
-    <t>bachelor</t>
-  </si>
-  <si>
-    <t>dep0001</t>
-  </si>
-  <si>
-    <t>business</t>
-  </si>
-  <si>
-    <t>dep0002</t>
-  </si>
-  <si>
-    <t>biology</t>
-  </si>
-  <si>
-    <t>master</t>
-  </si>
-  <si>
-    <t>tch0001</t>
-  </si>
-  <si>
     <t>Kate</t>
   </si>
   <si>
@@ -293,27 +198,12 @@
     <t>John</t>
   </si>
   <si>
-    <t>tch0002</t>
-  </si>
-  <si>
     <t>Hewitt</t>
   </si>
   <si>
-    <t>crs00001</t>
-  </si>
-  <si>
-    <t>data management</t>
-  </si>
-  <si>
     <t>Database management and SQL queries</t>
   </si>
   <si>
-    <t>crs00002</t>
-  </si>
-  <si>
-    <t>developmental biology</t>
-  </si>
-  <si>
     <t>Understanding life from conception to birth</t>
   </si>
   <si>
@@ -326,30 +216,15 @@
     <t>Einstein Science Building</t>
   </si>
   <si>
-    <t>clrmCSBR101</t>
-  </si>
-  <si>
-    <t>clrmESBR302</t>
-  </si>
-  <si>
     <t>Campus &amp; Online</t>
   </si>
   <si>
-    <t>sem2024SP</t>
-  </si>
-  <si>
     <t>Spring</t>
   </si>
   <si>
-    <t>sem2023AU</t>
-  </si>
-  <si>
     <t>Autumn</t>
   </si>
   <si>
-    <t>si000001</t>
-  </si>
-  <si>
     <t>Becky</t>
   </si>
   <si>
@@ -365,9 +240,6 @@
     <t>kate_hewitt@school.com</t>
   </si>
   <si>
-    <t>si000002</t>
-  </si>
-  <si>
     <t>George</t>
   </si>
   <si>
@@ -383,44 +255,227 @@
     <t>A-</t>
   </si>
   <si>
-    <t>grd0001</t>
-  </si>
-  <si>
-    <t>grd0002</t>
-  </si>
-  <si>
-    <t>reg000001</t>
-  </si>
-  <si>
-    <t>reg00002</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>bil000001</t>
-  </si>
-  <si>
-    <t>bil000101</t>
-  </si>
-  <si>
-    <t>Paid</t>
-  </si>
-  <si>
-    <t>Unpaid</t>
-  </si>
-  <si>
-    <t>sdg000001</t>
-  </si>
-  <si>
-    <t>sdg000002</t>
+    <t>Semester ID (PK) is composed of the year and season the course is (eg. 202404 --&gt; 2024 year, 01 = spring, 02 = summer, 03 = fall, 04 = winter)</t>
+  </si>
+  <si>
+    <t>Business Analytics</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Degree: Level - Will be constrained to a single character represting the level of degree (A = Associates, B = Bachelor, M = Masters, D = Doctorate)</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Data Management</t>
+  </si>
+  <si>
+    <t>Developmental Biology</t>
+  </si>
+  <si>
+    <t>Building Number</t>
+  </si>
+  <si>
+    <t>Classroom: Classroom_Id - Primary Key is composed of the building number and room number (5 digit, first 2 digits represent the building and last 3 indicate classroom)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student_Degree: Student_Degree_Id - Combination of Student_Id and Degree_Id </t>
+  </si>
+  <si>
+    <t>Data Considerations:</t>
+  </si>
+  <si>
+    <t>Degree_Name VARCHAR (100)</t>
+  </si>
+  <si>
+    <t>Level CHAR (1)</t>
+  </si>
+  <si>
+    <t>Department_Name VARCHAR (50)</t>
+  </si>
+  <si>
+    <t>Phone_Number VARCHAR (15)</t>
+  </si>
+  <si>
+    <t>Course_Id (PK) INTEGER</t>
+  </si>
+  <si>
+    <t>Degree_Id (PK) INTEGER</t>
+  </si>
+  <si>
+    <t>Department_Id (FK) INTEGER</t>
+  </si>
+  <si>
+    <t>Department_Id (PK) INTEGER</t>
+  </si>
+  <si>
+    <t>Degree_Id (FK) INTEGER</t>
+  </si>
+  <si>
+    <t>Course_Title VARCHAR (100)</t>
+  </si>
+  <si>
+    <t>Number_Credits INTEGER</t>
+  </si>
+  <si>
+    <t>Description VARCHAR (MAX)</t>
+  </si>
+  <si>
+    <t>Teacher_Id (FK) INTEGER</t>
+  </si>
+  <si>
+    <t>Classroom_Id (FK) INTEGER</t>
+  </si>
+  <si>
+    <t>Teacher_Id (PK) INTEGER</t>
+  </si>
+  <si>
+    <t>Teacher_First_Name VARCHAR (30)</t>
+  </si>
+  <si>
+    <t>Teacher_Last_Name VARCHAR (30)</t>
+  </si>
+  <si>
+    <t>Email VARCHAR (30)</t>
+  </si>
+  <si>
+    <t>801-222-1111</t>
+  </si>
+  <si>
+    <t>801-222-1112</t>
+  </si>
+  <si>
+    <t>801-222-1222</t>
+  </si>
+  <si>
+    <t>801-222-1223</t>
+  </si>
+  <si>
+    <t>801-223-0001</t>
+  </si>
+  <si>
+    <t>801-223-0002</t>
+  </si>
+  <si>
+    <t>Semester_Id (PK) INTEGER</t>
+  </si>
+  <si>
+    <t>Term_Availability VARCHAR (10)</t>
+  </si>
+  <si>
+    <t>Year INTEGER (4)</t>
+  </si>
+  <si>
+    <t>Classrom_Id (PK) INTEGER</t>
+  </si>
+  <si>
+    <t>Building_Name VARCHAR (50)</t>
+  </si>
+  <si>
+    <t>Capacity (INTEGER)</t>
+  </si>
+  <si>
+    <t>Classroom_Number CHAR (10)</t>
+  </si>
+  <si>
+    <t>Style CHAR (10)</t>
+  </si>
+  <si>
+    <t>Building Number INTEGER</t>
+  </si>
+  <si>
+    <t>Student_Id (PK) INTEGER</t>
+  </si>
+  <si>
+    <t>First_Name VARCHAR (30)</t>
+  </si>
+  <si>
+    <t>Last_Name VARCHAR (30)</t>
+  </si>
+  <si>
+    <t>Grade_Id (PK) CHAR (10)</t>
+  </si>
+  <si>
+    <t>Letter_Grade CHAR (2)</t>
+  </si>
+  <si>
+    <t>Numeric_Grade INTEGER</t>
+  </si>
+  <si>
+    <t>Registration_Id (PK) INTEGER</t>
+  </si>
+  <si>
+    <t>Student_Id (FK) INTEGER</t>
+  </si>
+  <si>
+    <t>Semester_Id (FK) INTEGER</t>
+  </si>
+  <si>
+    <t>Course_Id (FK) INTEGER</t>
+  </si>
+  <si>
+    <t>Letter_Grade (FK) CHAR (2)</t>
+  </si>
+  <si>
+    <t>Numeric_Grade (FK) INTEGER</t>
+  </si>
+  <si>
+    <t>Amount (FK) REAL</t>
+  </si>
+  <si>
+    <t>Billing_Id (PK) INTEGER</t>
+  </si>
+  <si>
+    <t>Amount REAL</t>
+  </si>
+  <si>
+    <t>Due_Date DATE</t>
+  </si>
+  <si>
+    <t>Payment_Date DATE</t>
+  </si>
+  <si>
+    <t>Status VARCHAR (15)</t>
+  </si>
+  <si>
+    <t>Student_Degree_Id (PK) INTEGER</t>
+  </si>
+  <si>
+    <t>Enrollment_Date DATE</t>
+  </si>
+  <si>
+    <t>Graduation_Date DATE</t>
+  </si>
+  <si>
+    <t>Data Modeling:</t>
+  </si>
+  <si>
+    <t>Use Underscores to denote spaces</t>
+  </si>
+  <si>
+    <t>PK/FK Built</t>
+  </si>
+  <si>
+    <t>Data Types Set</t>
+  </si>
+  <si>
+    <t>Numeric_Grade REAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,6 +495,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -515,7 +577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -523,14 +585,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -606,8 +674,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1217295</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>21166</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
@@ -615,7 +683,7 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>17145</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -630,12 +698,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1855470" y="2143125"/>
-          <a:ext cx="1857375" cy="1579245"/>
+          <a:off x="2677583" y="2131483"/>
+          <a:ext cx="2578312" cy="1562100"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 18718"/>
+            <a:gd name="adj1" fmla="val 24178"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -914,16 +982,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1199365</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21168</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>114436</xdr:rowOff>
+      <xdr:rowOff>105834</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>105104</xdr:colOff>
+      <xdr:colOff>103200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>131379</xdr:rowOff>
+      <xdr:rowOff>135190</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -938,12 +1006,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="3695572" y="2505539"/>
-          <a:ext cx="2498963" cy="384806"/>
+          <a:off x="6085418" y="2444751"/>
+          <a:ext cx="4601115" cy="389189"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 105770"/>
+            <a:gd name="adj1" fmla="val 107663"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1124,16 +1192,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1219254</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>94731</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1219255</xdr:colOff>
+      <xdr:rowOff>113109</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>17859</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>94731</xdr:rowOff>
+      <xdr:rowOff>113109</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1148,12 +1216,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8530513" y="3773352"/>
-          <a:ext cx="1221828" cy="183931"/>
+          <a:off x="14049375" y="3684984"/>
+          <a:ext cx="1827609" cy="178594"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 25886"/>
+            <a:gd name="adj1" fmla="val 27524"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1485,15 +1553,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>133116</xdr:colOff>
+      <xdr:colOff>166687</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>28612</xdr:rowOff>
+      <xdr:rowOff>29766</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>8474</xdr:colOff>
+      <xdr:colOff>10379</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>84674</xdr:rowOff>
+      <xdr:rowOff>86579</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1508,8 +1576,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8662073" y="2902441"/>
-          <a:ext cx="1094558" cy="594904"/>
+          <a:off x="14216062" y="2887266"/>
+          <a:ext cx="1653442" cy="592594"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1546,9 +1614,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>154021</xdr:colOff>
+      <xdr:colOff>202406</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>28372</xdr:rowOff>
+      <xdr:rowOff>29766</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1563,8 +1631,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="7494351" y="2936259"/>
-          <a:ext cx="1183532" cy="10411"/>
+          <a:off x="12733734" y="2875461"/>
+          <a:ext cx="1518047" cy="11805"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1690,15 +1758,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1218929</xdr:colOff>
+      <xdr:colOff>1803797</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>115661</xdr:rowOff>
+      <xdr:rowOff>113109</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>21772</xdr:colOff>
+      <xdr:colOff>17962</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>119743</xdr:rowOff>
+      <xdr:rowOff>115933</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1713,8 +1781,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9747886" y="1193347"/>
-          <a:ext cx="1241243" cy="183696"/>
+          <a:off x="15853172" y="1184672"/>
+          <a:ext cx="1797946" cy="181417"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1845,15 +1913,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>970462</xdr:colOff>
+      <xdr:colOff>1248834</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>83202</xdr:rowOff>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>172539</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>83202</xdr:rowOff>
+      <xdr:rowOff>85107</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1867,9 +1935,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="9503548" y="2658236"/>
-          <a:ext cx="423905" cy="0"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="15292917" y="2603500"/>
+          <a:ext cx="733455" cy="440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1895,15 +1963,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>981113</xdr:colOff>
+      <xdr:colOff>1241648</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>76285</xdr:rowOff>
+      <xdr:rowOff>82239</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>988188</xdr:colOff>
+      <xdr:colOff>1250628</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>57507</xdr:rowOff>
+      <xdr:rowOff>63461</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1918,8 +1986,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9514199" y="2651319"/>
-          <a:ext cx="7075" cy="716947"/>
+          <a:off x="15291023" y="2582552"/>
+          <a:ext cx="8980" cy="695597"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1945,15 +2013,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>988967</xdr:colOff>
+      <xdr:colOff>1248251</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>67886</xdr:rowOff>
+      <xdr:rowOff>65484</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>8981</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>79043</xdr:rowOff>
+      <xdr:rowOff>67389</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1967,9 +2035,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9522053" y="3378645"/>
-          <a:ext cx="241842" cy="11157"/>
+        <a:xfrm flipV="1">
+          <a:off x="15297626" y="3280172"/>
+          <a:ext cx="561499" cy="1905"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2098,7 +2166,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1045029</xdr:colOff>
+      <xdr:colOff>1666875</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>77833</xdr:rowOff>
     </xdr:from>
@@ -2106,7 +2174,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>237581</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
+      <xdr:rowOff>83343</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2121,8 +2189,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9573986" y="4568190"/>
-          <a:ext cx="2583452" cy="3810"/>
+          <a:off x="15716250" y="4542677"/>
+          <a:ext cx="3618956" cy="5510"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2148,15 +2216,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1052649</xdr:colOff>
+      <xdr:colOff>1658201</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>115931</xdr:rowOff>
+      <xdr:rowOff>94261</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1052649</xdr:colOff>
+      <xdr:colOff>1660922</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>77832</xdr:rowOff>
+      <xdr:rowOff>83343</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2170,9 +2238,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9585735" y="4346345"/>
-          <a:ext cx="0" cy="329763"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="15707576" y="4201917"/>
+          <a:ext cx="2721" cy="346270"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2198,15 +2266,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1044681</xdr:colOff>
+      <xdr:colOff>1661663</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>96225</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1210323</xdr:colOff>
+      <xdr:rowOff>102178</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>11840</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>96225</xdr:rowOff>
+      <xdr:rowOff>102178</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2221,8 +2289,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9577767" y="4326639"/>
-          <a:ext cx="165642" cy="0"/>
+          <a:off x="15711038" y="4209834"/>
+          <a:ext cx="159927" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2250,16 +2318,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1215258</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>21166</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>26276</xdr:rowOff>
+      <xdr:rowOff>28181</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>216776</xdr:colOff>
+      <xdr:colOff>218681</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>26276</xdr:rowOff>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2273,9 +2341,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1852448" y="3704897"/>
-          <a:ext cx="223345" cy="0"/>
+        <a:xfrm flipV="1">
+          <a:off x="2677583" y="3626514"/>
+          <a:ext cx="197515" cy="3569"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2789,6 +2857,1908 @@
         <a:xfrm flipH="1">
           <a:off x="9753600" y="1115786"/>
           <a:ext cx="157843" cy="5443"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Connector: Elbow 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08861AE1-093F-45FB-A899-5CEB6B93F147}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2752725" y="3779520"/>
+          <a:ext cx="1303020" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>21166</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>17145</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Connector: Elbow 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CA9CB43-37D3-4E48-9AC8-40DEF8BC34CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2770081" y="2143125"/>
+          <a:ext cx="3504989" cy="1571625"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 11635"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE115998-E4BA-4A11-9FA6-1A98F9E78169}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6265545" y="3722370"/>
+          <a:ext cx="259080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>265748</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>17009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>110898</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59CC861D-196E-427C-9E6D-DDB3E0D74709}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6523673" y="3097394"/>
+          <a:ext cx="10477" cy="636814"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BCA851-25C6-4E17-8E9A-78AA54425B32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4970145" y="3103245"/>
+          <a:ext cx="1554480" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>911678</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>105455</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD6425C4-675D-4BE0-86C5-F0C23077EF86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4963613" y="2275250"/>
+          <a:ext cx="0" cy="839425"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>902970</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>110096</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>110096</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B075C2D1-3C61-4AE3-93AF-36A43ACE7255}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="2285606"/>
+          <a:ext cx="1314450" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>21168</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>105834</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>103200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>135190</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Connector: Elbow 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00CF4097-8317-45A1-B560-27F15AE7194F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="6275283" y="2456604"/>
+          <a:ext cx="4602597" cy="393211"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 107663"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>131546</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>105456</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA876AD6-E660-402D-BA66-94183B9590CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10868025" y="2846171"/>
+          <a:ext cx="0" cy="695905"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>100263</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{258C222C-D1D7-45E2-AD83-A84E478F49F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10772775" y="3533775"/>
+          <a:ext cx="96453" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>956830</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>8660</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>11083</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>84167</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Connector: Elbow 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{980456DC-D434-448F-93B6-81F38BED6D93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13687945" y="3087140"/>
+          <a:ext cx="2447058" cy="618432"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>588819</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>8660</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>12989</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B904AE1B-CA6E-4C0A-82FB-B17F1C520C0C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="11361594" y="3087140"/>
+          <a:ext cx="2325831" cy="519"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>593182</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>86590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>593182</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>18704</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E8F2164-3D8D-4AC6-86CF-B9363DF87E77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="11362147" y="2256385"/>
+          <a:ext cx="0" cy="838894"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>183746</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>86071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>595572</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>94730</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82BE0C73-2830-4819-96D5-23AD57CE3CF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9106766" y="2255866"/>
+          <a:ext cx="2257771" cy="10564"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>189981</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>86591</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>86071</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE5C7A35-64DB-4C5C-AA1B-C1C535058893}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9114906" y="1351511"/>
+          <a:ext cx="519" cy="904355"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4330</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>90921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>194830</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A27DBBB-D49F-4BDF-88ED-8CA6CA4B66BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8925445" y="1361556"/>
+          <a:ext cx="190500" cy="519"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>166687</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>29766</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>10379</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>86579</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Connector: Elbow 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11955E37-084C-49B5-B49E-DA7F6FAC7B76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14486572" y="2923461"/>
+          <a:ext cx="1647727" cy="599738"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>17961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>202406</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>29766</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{383DCA6B-B77D-44E1-A29C-5C9A5C62DB4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="12925425" y="2913561"/>
+          <a:ext cx="1591151" cy="9900"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>125185</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>195943</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{911DE120-E157-403E-A0DE-90FB9DE7B1BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="12925425" y="1209130"/>
+          <a:ext cx="1633" cy="1704431"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>125185</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>195943</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>125185</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5AF2225-FB51-4603-AC47-93F0FE41CA49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12736558" y="1209130"/>
+          <a:ext cx="190500" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>17962</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>115933</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Connector: Elbow 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01730A63-CF4A-491A-A9D4-82E402A68A4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14639925" y="1019175"/>
+          <a:ext cx="1818187" cy="182608"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>167095</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>166823</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>167095</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5752D2B0-A0B2-48AA-87A9-37DE5282997C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16134805" y="1256755"/>
+          <a:ext cx="161653" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>168729</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>170906</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>94706</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B32CCA5-82F0-48FE-A3C7-F79D99135114}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16298364" y="1247230"/>
+          <a:ext cx="0" cy="1381126"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1248834</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>172539</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>85107</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E2E5D48-7D07-4BB2-A58A-63316573E1C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="15563004" y="2620222"/>
+          <a:ext cx="735360" cy="440"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1241648</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>82239</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1250628</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>63461</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Connector 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82413937-CE19-4F6F-A362-6BDB100B6355}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15553913" y="2617794"/>
+          <a:ext cx="10885" cy="705122"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1248251</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>65484</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>67389</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Arrow Connector 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0104C99C-E210-49C0-A720-295F4F8BF797}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="15562421" y="3324939"/>
+          <a:ext cx="563404" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>21166</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28181</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>218681</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC371FE2-7CD4-409D-80E6-11AE41DE2446}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2770081" y="3649586"/>
+          <a:ext cx="203230" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>216776</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>52551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>216776</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>32845</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78A01D96-FE77-46BD-81A9-313B8947AFE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2971406" y="3132936"/>
+          <a:ext cx="0" cy="523219"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>59120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>229914</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>65689</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Connector 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD5C4DB0-460B-462D-8626-81DB398C1041}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="381000" y="3131885"/>
+          <a:ext cx="2601639" cy="12284"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>374431</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>118242</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>387569</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>78827</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Connector 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D66039B-402B-41C9-9E9B-BD362722814A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="372526" y="2105157"/>
+          <a:ext cx="16948" cy="1046435"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>387569</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>111673</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6569</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>118242</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Straight Arrow Connector 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AB03E66-A506-4FC1-A49E-A0CAD2A9A9CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="389474" y="2106208"/>
+          <a:ext cx="257175" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>262759</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>157655</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1095113</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>94725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Connector: Elbow 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A6531E8-A081-4AA5-ABF6-AE40BA021275}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3019294" y="515795"/>
+          <a:ext cx="17613499" cy="483805"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 97969"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>141514</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Connector: Elbow 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAFCA070-DDBF-4C78-8EFB-20309DEE4739}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16269244" y="725533"/>
+          <a:ext cx="4371431" cy="463516"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 87366"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>272143</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>293915</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Connector 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{317354F0-414D-4D67-9E3F-DFC1997C74D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3021058" y="514350"/>
+          <a:ext cx="27487" cy="1038770"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>293915</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>103415</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Connector 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F80D6C23-D26B-4B5A-8D5D-0119D8E30302}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2754358" y="1553120"/>
+          <a:ext cx="294187" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>141514</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>146957</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Straight Connector 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{021AA715-4D44-4E06-8B50-4D2D7E9ECAF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16269244" y="725533"/>
+          <a:ext cx="7348" cy="398417"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>5443</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Straight Connector 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68DA78C5-23CA-43F1-9FC7-C76281E0A448}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="16127458" y="1123950"/>
+          <a:ext cx="159748" cy="1633"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3131,23 +5101,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB87B99-C53A-4003-A685-AB05DF1DCFCE}">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3:U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="16.7890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.62890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.47265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="16.7890625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.62890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.47265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.15625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.89453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.62890625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.3125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.3125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.83984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.7890625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.734375" customWidth="1"/>
     <col min="16" max="16" width="10.20703125" bestFit="1" customWidth="1"/>
@@ -3157,22 +5130,22 @@
     <col min="22" max="22" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="M4" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="M4" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="M5" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="G6" s="4" t="s">
         <v>5</v>
       </c>
@@ -3183,119 +5156,116 @@
         <v>8</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>46</v>
+        <v>131</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1"/>
       <c r="E8" s="3" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>23</v>
+        <v>110</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>59</v>
+        <v>137</v>
       </c>
       <c r="O8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="S8" s="1"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>12</v>
+        <v>132</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="5" t="s">
-        <v>22</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="9"/>
-      <c r="K12" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>91</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+        <v>97</v>
+      </c>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="E14" s="2" t="s">
-        <v>32</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -3305,18 +5275,18 @@
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="J18" s="3" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="F19" s="4" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>6</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -3328,87 +5298,90 @@
         <v>2</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>39</v>
+        <v>112</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="3" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>43</v>
+        <v>122</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>87</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="5" t="s">
-        <v>27</v>
+      <c r="B23" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="D24" s="7" t="s">
-        <v>15</v>
+      <c r="D24" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>17</v>
+        <v>116</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="D25" s="5" t="s">
-        <v>9</v>
+      <c r="D25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="D26" s="5" t="s">
-        <v>27</v>
+      <c r="D26" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J30" t="s">
         <v>7</v>
@@ -3416,89 +5389,89 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
         <v>19</v>
       </c>
-      <c r="D31" t="s">
+      <c r="J31" t="s">
+        <v>45</v>
+      </c>
+      <c r="K31" t="s">
         <v>20</v>
       </c>
-      <c r="E31" t="s">
+      <c r="L31" t="s">
         <v>21</v>
-      </c>
-      <c r="J31" t="s">
-        <v>67</v>
-      </c>
-      <c r="K31" t="s">
-        <v>23</v>
-      </c>
-      <c r="L31" t="s">
-        <v>24</v>
       </c>
       <c r="M31" t="s">
         <v>9</v>
       </c>
       <c r="N31" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" t="s">
-        <v>72</v>
+      <c r="B32">
+        <v>10001</v>
       </c>
       <c r="C32" t="s">
         <v>74</v>
       </c>
       <c r="D32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32">
+        <v>10001</v>
+      </c>
+      <c r="J32">
+        <v>500001</v>
+      </c>
+      <c r="K32" t="s">
+        <v>62</v>
+      </c>
+      <c r="L32" t="s">
+        <v>63</v>
+      </c>
+      <c r="M32" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="N32" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33">
+        <v>10002</v>
+      </c>
+      <c r="C33" t="s">
         <v>75</v>
       </c>
-      <c r="E32" t="s">
+      <c r="D33" t="s">
         <v>76</v>
       </c>
-      <c r="J32" t="s">
-        <v>103</v>
-      </c>
-      <c r="K32" t="s">
-        <v>104</v>
-      </c>
-      <c r="L32" t="s">
-        <v>105</v>
-      </c>
-      <c r="M32" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="N32">
-        <v>8012230001</v>
-      </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" t="s">
-        <v>80</v>
-      </c>
-      <c r="E33" t="s">
-        <v>78</v>
-      </c>
-      <c r="J33" t="s">
-        <v>109</v>
+      <c r="E33">
+        <v>30002</v>
+      </c>
+      <c r="J33">
+        <v>385269</v>
       </c>
       <c r="K33" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="L33" t="s">
-        <v>111</v>
-      </c>
-      <c r="M33" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="N33">
-        <v>8012230002</v>
+        <v>68</v>
+      </c>
+      <c r="M33" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="N33" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.55000000000000004">
@@ -3511,59 +5484,59 @@
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D36" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J36" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="K36" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="L36" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B37" t="s">
-        <v>76</v>
+      <c r="B37">
+        <v>10001</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37">
-        <v>8012221111</v>
-      </c>
-      <c r="J37" t="s">
-        <v>115</v>
+        <v>78</v>
+      </c>
+      <c r="D37" t="s">
+        <v>103</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
       </c>
       <c r="K37" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="L37">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B38" t="s">
-        <v>78</v>
+      <c r="B38">
+        <v>30002</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38">
-        <v>8012221112</v>
-      </c>
-      <c r="J38" t="s">
-        <v>116</v>
+        <v>75</v>
+      </c>
+      <c r="D38" t="s">
+        <v>104</v>
+      </c>
+      <c r="J38">
+        <v>2</v>
       </c>
       <c r="K38" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="L38">
         <v>3.8</v>
@@ -3579,78 +5552,78 @@
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D41" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E41" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F41" t="s">
         <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J41" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="K41" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="L41" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="M41" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="N41" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="O41" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="P41" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" t="s">
-        <v>81</v>
+      <c r="B42">
+        <v>2001</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="D42" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42" t="s">
-        <v>76</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="G42">
-        <v>8012221222</v>
-      </c>
-      <c r="J42" t="s">
-        <v>117</v>
-      </c>
-      <c r="K42" t="s">
-        <v>103</v>
-      </c>
-      <c r="L42" t="s">
-        <v>99</v>
-      </c>
-      <c r="M42" t="s">
-        <v>87</v>
+        <v>51</v>
+      </c>
+      <c r="E42">
+        <v>10001</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" t="s">
+        <v>105</v>
+      </c>
+      <c r="J42">
+        <v>100001</v>
+      </c>
+      <c r="K42">
+        <v>500001</v>
+      </c>
+      <c r="L42">
+        <v>202401</v>
+      </c>
+      <c r="M42">
+        <v>15082</v>
       </c>
       <c r="N42" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="O42">
         <v>4</v>
@@ -3660,38 +5633,38 @@
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43" t="s">
-        <v>85</v>
+      <c r="B43">
+        <v>2002</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="D43" t="s">
-        <v>86</v>
-      </c>
-      <c r="E43" t="s">
-        <v>78</v>
-      </c>
-      <c r="F43" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="G43">
-        <v>8012221223</v>
-      </c>
-      <c r="J43" t="s">
-        <v>118</v>
-      </c>
-      <c r="K43" t="s">
-        <v>109</v>
-      </c>
-      <c r="L43" t="s">
-        <v>101</v>
-      </c>
-      <c r="M43" t="s">
-        <v>90</v>
+        <v>53</v>
+      </c>
+      <c r="E43">
+        <v>30002</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G43" t="s">
+        <v>106</v>
+      </c>
+      <c r="J43">
+        <v>100002</v>
+      </c>
+      <c r="K43">
+        <v>385269</v>
+      </c>
+      <c r="L43">
+        <v>202303</v>
+      </c>
+      <c r="M43">
+        <v>21543</v>
       </c>
       <c r="N43" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="O43">
         <v>3.1</v>
@@ -3710,164 +5683,173 @@
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E46" t="s">
         <v>14</v>
       </c>
       <c r="F46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G46" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="H46" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="J46" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="K46" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="L46" t="s">
         <v>12</v>
       </c>
       <c r="M46" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="N46" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="O46" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B47" t="s">
-        <v>87</v>
+      <c r="B47">
+        <v>15082</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D47">
         <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>89</v>
-      </c>
-      <c r="F47" t="s">
-        <v>72</v>
-      </c>
-      <c r="G47" t="s">
-        <v>81</v>
-      </c>
-      <c r="J47" t="s">
-        <v>120</v>
-      </c>
-      <c r="K47" t="s">
-        <v>103</v>
+        <v>54</v>
+      </c>
+      <c r="F47">
+        <v>10001</v>
+      </c>
+      <c r="G47">
+        <v>2001</v>
+      </c>
+      <c r="H47">
+        <v>3101</v>
+      </c>
+      <c r="J47">
+        <v>100000</v>
+      </c>
+      <c r="K47">
+        <v>500001</v>
       </c>
       <c r="L47">
         <v>3432</v>
       </c>
-      <c r="M47" s="11">
+      <c r="M47" s="9">
         <v>44941</v>
       </c>
-      <c r="N47" s="11">
+      <c r="N47" s="9">
         <v>44940</v>
       </c>
-      <c r="O47" t="s">
-        <v>122</v>
+      <c r="O47">
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B48" t="s">
-        <v>90</v>
+      <c r="B48">
+        <v>21543</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D48">
         <v>3</v>
       </c>
       <c r="E48" t="s">
-        <v>92</v>
-      </c>
-      <c r="F48" t="s">
-        <v>73</v>
-      </c>
-      <c r="G48" t="s">
-        <v>85</v>
-      </c>
-      <c r="J48" t="s">
-        <v>121</v>
-      </c>
-      <c r="K48" t="s">
-        <v>103</v>
+        <v>55</v>
+      </c>
+      <c r="F48">
+        <v>30002</v>
+      </c>
+      <c r="G48">
+        <v>2002</v>
+      </c>
+      <c r="H48">
+        <v>2302</v>
+      </c>
+      <c r="J48">
+        <v>100001</v>
+      </c>
+      <c r="K48">
+        <v>385269</v>
       </c>
       <c r="L48">
         <v>3432</v>
       </c>
-      <c r="M48" s="11">
+      <c r="M48" s="9">
         <v>45672</v>
       </c>
-      <c r="O48" t="s">
-        <v>123</v>
+      <c r="O48">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="J50" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="C51" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D51" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E51" t="s">
         <v>10</v>
       </c>
       <c r="F51" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="G51" t="s">
+        <v>81</v>
       </c>
       <c r="J51" t="s">
+        <v>36</v>
+      </c>
+      <c r="K51" t="s">
+        <v>39</v>
+      </c>
+      <c r="L51" t="s">
+        <v>45</v>
+      </c>
+      <c r="M51" t="s">
+        <v>37</v>
+      </c>
+      <c r="N51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B52">
+        <v>3101</v>
+      </c>
+      <c r="C52" t="s">
         <v>56</v>
-      </c>
-      <c r="K51" t="s">
-        <v>61</v>
-      </c>
-      <c r="L51" t="s">
-        <v>67</v>
-      </c>
-      <c r="M51" t="s">
-        <v>59</v>
-      </c>
-      <c r="N51" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B52" t="s">
-        <v>96</v>
-      </c>
-      <c r="C52" t="s">
-        <v>93</v>
       </c>
       <c r="D52">
         <v>101</v>
@@ -3876,30 +5858,33 @@
         <v>54</v>
       </c>
       <c r="F52" t="s">
-        <v>94</v>
-      </c>
-      <c r="J52" t="s">
-        <v>124</v>
-      </c>
-      <c r="K52" t="s">
-        <v>72</v>
-      </c>
-      <c r="L52" t="s">
-        <v>103</v>
-      </c>
-      <c r="M52" s="11">
+        <v>57</v>
+      </c>
+      <c r="G52">
+        <v>3</v>
+      </c>
+      <c r="J52">
+        <v>50000110001</v>
+      </c>
+      <c r="K52">
+        <v>10001</v>
+      </c>
+      <c r="L52">
+        <v>500001</v>
+      </c>
+      <c r="M52" s="9">
         <v>44927</v>
       </c>
-      <c r="N52" s="11">
+      <c r="N52" s="9">
         <v>46737</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53" t="s">
-        <v>97</v>
+      <c r="B53">
+        <v>2302</v>
       </c>
       <c r="C53" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="D53">
         <v>302</v>
@@ -3908,21 +5893,24 @@
         <v>32</v>
       </c>
       <c r="F53" t="s">
-        <v>98</v>
-      </c>
-      <c r="J53" t="s">
-        <v>125</v>
-      </c>
-      <c r="K53" t="s">
-        <v>73</v>
-      </c>
-      <c r="L53" t="s">
-        <v>109</v>
-      </c>
-      <c r="M53" s="11">
+        <v>59</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="J53">
+        <v>38526930002</v>
+      </c>
+      <c r="K53">
+        <v>10002</v>
+      </c>
+      <c r="L53">
+        <v>385269</v>
+      </c>
+      <c r="M53" s="9">
         <v>44713</v>
       </c>
-      <c r="N53" s="11">
+      <c r="N53" s="9">
         <v>46143</v>
       </c>
     </row>
@@ -3933,32 +5921,32 @@
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B57" t="s">
-        <v>99</v>
+      <c r="B57">
+        <v>202401</v>
       </c>
       <c r="C57" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D57">
         <v>2024</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="B58" t="s">
-        <v>101</v>
+      <c r="B58">
+        <v>202303</v>
       </c>
       <c r="C58" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="D58">
         <v>2023</v>
@@ -3975,4 +5963,321 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
   <drawing r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE5ECE1-46ED-4217-AACC-5D35248B0C41}">
+  <dimension ref="B3:M42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.05078125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.68359375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.83984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.68359375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.26171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.1015625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.05078125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1015625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.47265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M4" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="E7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="E13" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="J16" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="J17" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="14"/>
+      <c r="J18" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" s="15"/>
+      <c r="J19" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="J20" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="J21" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="J22" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D23" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H24" s="16"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" s="16"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H26" s="16"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="H27" s="16"/>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D34" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C36" s="1"/>
+      <c r="D36" t="s">
+        <v>141</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D38" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>